<commit_message>
Printed almost all barcodes, all the registered books have barcodes
</commit_message>
<xml_diff>
--- a/activity_history.xlsx
+++ b/activity_history.xlsx
@@ -461,7 +461,7 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Barcode</t>
+          <t>NSS Barcode</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
@@ -488,17 +488,17 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>registered</t>
+          <t>Registered</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>17.04.2025 19:08:43</t>
+          <t>01.05.2025 20:26:57</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>9780672319242-1</t>
+          <t>9780672319242+1</t>
         </is>
       </c>
       <c r="G2" t="inlineStr"/>
@@ -521,17 +521,17 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>registered</t>
+          <t>Registered</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>17.04.2025 19:08:43</t>
+          <t>01.05.2025 20:26:57</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>9781932394757-1</t>
+          <t>9781932394757+1</t>
         </is>
       </c>
       <c r="G3" t="inlineStr"/>
@@ -554,17 +554,17 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>registered</t>
+          <t>Registered</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>17.04.2025 19:08:44</t>
+          <t>01.05.2025 20:26:58</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>9780201776416-1</t>
+          <t>9780201776416+1</t>
         </is>
       </c>
       <c r="G4" t="inlineStr"/>
@@ -587,17 +587,17 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>registered</t>
+          <t>Registered</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>17.04.2025 19:08:45</t>
+          <t>01.05.2025 20:26:59</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>9780130282293-1</t>
+          <t>9780130282293+1</t>
         </is>
       </c>
       <c r="G5" t="inlineStr"/>
@@ -620,17 +620,17 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>registered</t>
+          <t>Registered</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>17.04.2025 19:08:46</t>
+          <t>01.05.2025 20:27:00</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>9780321150400-1</t>
+          <t>9780321150400+1</t>
         </is>
       </c>
       <c r="G6" t="inlineStr"/>
@@ -653,17 +653,17 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>registered</t>
+          <t>Registered</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>17.04.2025 19:08:46</t>
+          <t>01.05.2025 20:27:01</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>9780137056323-1</t>
+          <t>9780137056323+1</t>
         </is>
       </c>
       <c r="G7" t="inlineStr"/>
@@ -686,17 +686,17 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>registered</t>
+          <t>Registered</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>17.04.2025 19:08:47</t>
+          <t>01.05.2025 20:27:02</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>9780130914491-1</t>
+          <t>9780130914491+1</t>
         </is>
       </c>
       <c r="G8" t="inlineStr"/>
@@ -719,17 +719,17 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>registered</t>
+          <t>Registered</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>17.04.2025 19:08:47</t>
+          <t>01.05.2025 20:27:03</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>9780131668362-1</t>
+          <t>9780131668362+1</t>
         </is>
       </c>
       <c r="G9" t="inlineStr"/>
@@ -752,17 +752,17 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>registered</t>
+          <t>Registered</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>17.04.2025 19:08:48</t>
+          <t>01.05.2025 20:27:04</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>9781565925120-1</t>
+          <t>9781565925120+1</t>
         </is>
       </c>
       <c r="G10" t="inlineStr"/>
@@ -785,17 +785,17 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>registered</t>
+          <t>Registered</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>17.04.2025 19:08:48</t>
+          <t>01.05.2025 20:27:05</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>9781565923225-1</t>
+          <t>9781565923225+1</t>
         </is>
       </c>
       <c r="G11" t="inlineStr"/>
@@ -818,17 +818,17 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>registered</t>
+          <t>Registered</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>17.04.2025 19:08:49</t>
+          <t>01.05.2025 20:27:05</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>9780137081301-1</t>
+          <t>9780137081301+1</t>
         </is>
       </c>
       <c r="G12" t="inlineStr"/>
@@ -851,17 +851,17 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>registered</t>
+          <t>Registered</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>17.04.2025 19:08:49</t>
+          <t>01.05.2025 20:27:07</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>9780130083968-1</t>
+          <t>9780130083968+1</t>
         </is>
       </c>
       <c r="G13" t="inlineStr"/>
@@ -884,17 +884,17 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>registered</t>
+          <t>Registered</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>17.04.2025 19:08:50</t>
+          <t>01.05.2025 20:27:08</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>9780471262725-1</t>
+          <t>9780471262725+1</t>
         </is>
       </c>
       <c r="G14" t="inlineStr"/>
@@ -917,17 +917,17 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>registered</t>
+          <t>Registered</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>17.04.2025 19:08:50</t>
+          <t>01.05.2025 20:27:09</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>9780321702012-1</t>
+          <t>9780321702012+1</t>
         </is>
       </c>
       <c r="G15" t="inlineStr"/>
@@ -950,17 +950,17 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>registered</t>
+          <t>Registered</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>17.04.2025 19:08:51</t>
+          <t>01.05.2025 20:27:10</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>9780131211919-1</t>
+          <t>9780131211919+1</t>
         </is>
       </c>
       <c r="G16" t="inlineStr"/>
@@ -983,17 +983,17 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>registered</t>
+          <t>Registered</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>17.04.2025 19:08:52</t>
+          <t>01.05.2025 20:27:11</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>9781597496551-1</t>
+          <t>9781597496551+1</t>
         </is>
       </c>
       <c r="G17" t="inlineStr"/>
@@ -1016,17 +1016,17 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>registered</t>
+          <t>Registered</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>17.04.2025 19:08:52</t>
+          <t>01.05.2025 20:27:12</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>9780130474582-1</t>
+          <t>9780130474582+1</t>
         </is>
       </c>
       <c r="G18" t="inlineStr"/>
@@ -1049,17 +1049,17 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>registered</t>
+          <t>Registered</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>17.04.2025 19:08:53</t>
+          <t>01.05.2025 20:27:12</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>9780131365896-1</t>
+          <t>9780131365896+1</t>
         </is>
       </c>
       <c r="G19" t="inlineStr"/>
@@ -1082,17 +1082,17 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>registered</t>
+          <t>Registered</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>17.04.2025 19:08:53</t>
+          <t>01.05.2025 20:27:13</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>9780321245748-1</t>
+          <t>9780321245748+1</t>
         </is>
       </c>
       <c r="G20" t="inlineStr"/>
@@ -1115,17 +1115,17 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>registered</t>
+          <t>Registered</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>17.04.2025 19:08:54</t>
+          <t>01.05.2025 20:27:14</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>9780201485394-1</t>
+          <t>9780201485394+1</t>
         </is>
       </c>
       <c r="G21" t="inlineStr"/>
@@ -1148,17 +1148,17 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>registered</t>
+          <t>Registered</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>17.04.2025 19:08:55</t>
+          <t>01.05.2025 20:27:15</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>9780201593990-1</t>
+          <t>9780201593990+1</t>
         </is>
       </c>
       <c r="G22" t="inlineStr"/>
@@ -1181,17 +1181,17 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>registered</t>
+          <t>Registered</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>17.04.2025 19:08:56</t>
+          <t>01.05.2025 20:27:16</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>9781292223858-1</t>
+          <t>9781292223858+1</t>
         </is>
       </c>
       <c r="G23" t="inlineStr"/>
@@ -1214,17 +1214,17 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>registered</t>
+          <t>Registered</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>17.04.2025 19:08:57</t>
+          <t>01.05.2025 20:27:17</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>9780201175493-1</t>
+          <t>9780201175493+1</t>
         </is>
       </c>
       <c r="G24" t="inlineStr"/>
@@ -1247,17 +1247,17 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>registered</t>
+          <t>Registered</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>17.04.2025 19:08:57</t>
+          <t>01.05.2025 20:27:18</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>9781292109220-1</t>
+          <t>9781292109220+1</t>
         </is>
       </c>
       <c r="G25" t="inlineStr"/>
@@ -1280,17 +1280,17 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>registered</t>
+          <t>Registered</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>17.04.2025 19:08:58</t>
+          <t>01.05.2025 20:27:19</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>9780135075807-1</t>
+          <t>9780135075807+1</t>
         </is>
       </c>
       <c r="G26" t="inlineStr"/>
@@ -1313,17 +1313,17 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>registered</t>
+          <t>Registered</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>17.04.2025 19:08:58</t>
+          <t>01.05.2025 20:27:21</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>9780131489530-1</t>
+          <t>9780131489530+1</t>
         </is>
       </c>
       <c r="G27" t="inlineStr"/>
@@ -1346,17 +1346,17 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>registered</t>
+          <t>Registered</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>17.04.2025 19:08:59</t>
+          <t>01.05.2025 20:27:21</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>9781259060489-1</t>
+          <t>9781259060489+1</t>
         </is>
       </c>
       <c r="G28" t="inlineStr"/>
@@ -1379,17 +1379,17 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>registered</t>
+          <t>Registered</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>17.04.2025 19:08:59</t>
+          <t>01.05.2025 20:27:22</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>9780321549358-1</t>
+          <t>9780321549358+1</t>
         </is>
       </c>
       <c r="G29" t="inlineStr"/>
@@ -1412,17 +1412,17 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>registered</t>
+          <t>Registered</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>17.04.2025 19:09:00</t>
+          <t>01.05.2025 20:27:23</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>9780321549341-1</t>
+          <t>9780321549341+1</t>
         </is>
       </c>
       <c r="G30" t="inlineStr"/>
@@ -1445,17 +1445,17 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>registered</t>
+          <t>Registered</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>17.04.2025 19:09:01</t>
+          <t>01.05.2025 20:27:24</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>9780805331592-1</t>
+          <t>9780805331592+1</t>
         </is>
       </c>
       <c r="G31" t="inlineStr"/>
@@ -1478,17 +1478,17 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>registered</t>
+          <t>Registered</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>17.04.2025 19:09:01</t>
+          <t>01.05.2025 20:27:24</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>9780805300604-1</t>
+          <t>9780805300604+1</t>
         </is>
       </c>
       <c r="G32" t="inlineStr"/>
@@ -1511,17 +1511,17 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>registered</t>
+          <t>Registered</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>17.04.2025 19:09:02</t>
+          <t>01.05.2025 20:27:25</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>9780201590630-1</t>
+          <t>9780201590630+1</t>
         </is>
       </c>
       <c r="G33" t="inlineStr"/>
@@ -1544,17 +1544,17 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>registered</t>
+          <t>Registered</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>17.04.2025 19:09:03</t>
+          <t>01.05.2025 20:27:26</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>9781118794753-1</t>
+          <t>9781118794753+1</t>
         </is>
       </c>
       <c r="G34" t="inlineStr"/>
@@ -1577,17 +1577,17 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>registered</t>
+          <t>Registered</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>17.04.2025 19:09:04</t>
+          <t>01.05.2025 20:27:27</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>9780321417206-1</t>
+          <t>9780321417206+1</t>
         </is>
       </c>
       <c r="G35" t="inlineStr"/>
@@ -1610,17 +1610,17 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>registered</t>
+          <t>Registered</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>17.04.2025 19:09:04</t>
+          <t>01.05.2025 20:27:28</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>9781430265290-1</t>
+          <t>9781430265290+1</t>
         </is>
       </c>
       <c r="G36" t="inlineStr"/>
@@ -1643,17 +1643,17 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>registered</t>
+          <t>Registered</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>17.04.2025 19:09:05</t>
+          <t>01.05.2025 20:27:28</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>9780131986190-1</t>
+          <t>9780131986190+1</t>
         </is>
       </c>
       <c r="G37" t="inlineStr"/>
@@ -1676,17 +1676,17 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>registered</t>
+          <t>Registered</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>17.04.2025 19:09:05</t>
+          <t>01.05.2025 20:27:29</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>9780805353822-1</t>
+          <t>9780805353822+1</t>
         </is>
       </c>
       <c r="G38" t="inlineStr"/>
@@ -1709,17 +1709,17 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>registered</t>
+          <t>Registered</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>17.04.2025 19:09:06</t>
+          <t>01.05.2025 20:27:30</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>9780596003234-1</t>
+          <t>9780596003234+1</t>
         </is>
       </c>
       <c r="G39" t="inlineStr"/>
@@ -1742,17 +1742,17 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>registered</t>
+          <t>Registered</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>17.04.2025 19:09:06</t>
+          <t>01.05.2025 20:27:31</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>9780201845594-1</t>
+          <t>9780201845594+1</t>
         </is>
       </c>
       <c r="G40" t="inlineStr"/>
@@ -1775,17 +1775,17 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>registered</t>
+          <t>Registered</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>17.04.2025 19:09:07</t>
+          <t>01.05.2025 20:27:32</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>9781584503309-1</t>
+          <t>9781584503309+1</t>
         </is>
       </c>
       <c r="G41" t="inlineStr"/>
@@ -1808,17 +1808,17 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>registered</t>
+          <t>Registered</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>17.04.2025 19:09:07</t>
+          <t>01.05.2025 20:27:33</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>9780471599609-1</t>
+          <t>9780471599609+1</t>
         </is>
       </c>
       <c r="G42" t="inlineStr"/>
@@ -1841,17 +1841,17 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>registered</t>
+          <t>Registered</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>17.04.2025 19:09:08</t>
+          <t>01.05.2025 20:27:34</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>9780131489066-1</t>
+          <t>9780131489066+1</t>
         </is>
       </c>
       <c r="G43" t="inlineStr"/>
@@ -1874,17 +1874,17 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>registered</t>
+          <t>Registered</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>17.04.2025 19:09:08</t>
+          <t>01.05.2025 20:27:35</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>9780201715941-1</t>
+          <t>9780201715941+1</t>
         </is>
       </c>
       <c r="G44" t="inlineStr"/>
@@ -1907,17 +1907,17 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>registered</t>
+          <t>Registered</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>17.04.2025 19:09:09</t>
+          <t>01.05.2025 20:27:36</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>9781292110653-1</t>
+          <t>9781292110653+1</t>
         </is>
       </c>
       <c r="G45" t="inlineStr"/>
@@ -1940,17 +1940,17 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>registered</t>
+          <t>Registered</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>17.04.2025 19:09:09</t>
+          <t>01.05.2025 20:27:37</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>9780321312556-1</t>
+          <t>9780321312556+1</t>
         </is>
       </c>
       <c r="G46" t="inlineStr"/>
@@ -1973,17 +1973,17 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>registered</t>
+          <t>Registered</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>17.04.2025 19:09:10</t>
+          <t>01.05.2025 20:27:38</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>9780273751472-1</t>
+          <t>9780273751472+1</t>
         </is>
       </c>
       <c r="G47" t="inlineStr"/>
@@ -2006,17 +2006,17 @@
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>registered</t>
+          <t>Registered</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>17.04.2025 19:09:11</t>
+          <t>01.05.2025 20:27:40</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>9780132222204-1</t>
+          <t>9780132222204+1</t>
         </is>
       </c>
       <c r="G48" t="inlineStr"/>
@@ -2039,17 +2039,17 @@
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>registered</t>
+          <t>Registered</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>17.04.2025 19:09:11</t>
+          <t>01.05.2025 20:27:40</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>9780321601667-1</t>
+          <t>9780321601667+1</t>
         </is>
       </c>
       <c r="G49" t="inlineStr"/>
@@ -2072,17 +2072,17 @@
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>registered</t>
+          <t>Registered</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>17.04.2025 19:09:12</t>
+          <t>01.05.2025 20:27:41</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>9780132150705-1</t>
+          <t>9780132150705+1</t>
         </is>
       </c>
       <c r="G50" t="inlineStr"/>
@@ -2105,17 +2105,17 @@
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>registered</t>
+          <t>Registered</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>17.04.2025 19:09:12</t>
+          <t>01.05.2025 20:27:43</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>9780130266118-1</t>
+          <t>9780130266118+1</t>
         </is>
       </c>
       <c r="G51" t="inlineStr"/>
@@ -2138,17 +2138,17 @@
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>registered</t>
+          <t>Registered</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>17.04.2025 19:09:13</t>
+          <t>01.05.2025 20:27:44</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>9780321269812-1</t>
+          <t>9780321269812+1</t>
         </is>
       </c>
       <c r="G52" t="inlineStr"/>
@@ -2171,17 +2171,17 @@
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>registered</t>
+          <t>Registered</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>17.04.2025 19:09:13</t>
+          <t>01.05.2025 20:27:45</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>9780321687296-1</t>
+          <t>9780321687296+1</t>
         </is>
       </c>
       <c r="G53" t="inlineStr"/>
@@ -2204,17 +2204,17 @@
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>registered</t>
+          <t>Registered</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>17.04.2025 19:09:14</t>
+          <t>01.05.2025 20:27:46</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>9780672325618-1</t>
+          <t>9780672325618+1</t>
         </is>
       </c>
       <c r="G54" t="inlineStr"/>
@@ -2237,17 +2237,17 @@
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>registered</t>
+          <t>Registered</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>17.04.2025 19:09:15</t>
+          <t>01.05.2025 20:27:47</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>9788205302563-1</t>
+          <t>9788205302563+1</t>
         </is>
       </c>
       <c r="G55" t="inlineStr"/>
@@ -2270,17 +2270,17 @@
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>registered</t>
+          <t>Registered</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>17.04.2025 19:09:15</t>
+          <t>01.05.2025 20:27:48</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>9780672337109-1</t>
+          <t>9780672337109+1</t>
         </is>
       </c>
       <c r="G56" t="inlineStr"/>
@@ -2303,17 +2303,17 @@
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>registered</t>
+          <t>Registered</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>17.04.2025 19:09:16</t>
+          <t>01.05.2025 20:27:49</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>9780984782857-1</t>
+          <t>9780984782857+1</t>
         </is>
       </c>
       <c r="G57" t="inlineStr"/>
@@ -2336,17 +2336,17 @@
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>registered</t>
+          <t>Registered</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>17.04.2025 19:09:17</t>
+          <t>01.05.2025 20:27:51</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>9780764543982-1</t>
+          <t>9780764543982+1</t>
         </is>
       </c>
       <c r="G58" t="inlineStr"/>
@@ -2369,17 +2369,17 @@
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>registered</t>
+          <t>Registered</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>17.04.2025 19:09:18</t>
+          <t>01.05.2025 20:27:52</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>9781576761618-1</t>
+          <t>9781576761618+1</t>
         </is>
       </c>
       <c r="G59" t="inlineStr"/>
@@ -2402,17 +2402,17 @@
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>registered</t>
+          <t>Registered</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>17.04.2025 19:09:19</t>
+          <t>01.05.2025 20:27:53</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>9780132465403-1</t>
+          <t>9780132465403+1</t>
         </is>
       </c>
       <c r="G60" t="inlineStr"/>
@@ -2435,17 +2435,17 @@
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>registered</t>
+          <t>Registered</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>17.04.2025 19:09:20</t>
+          <t>01.05.2025 20:27:54</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>9780321584106-1</t>
+          <t>9780321584106+1</t>
         </is>
       </c>
       <c r="G61" t="inlineStr"/>
@@ -2468,17 +2468,17 @@
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>registered</t>
+          <t>Registered</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>17.04.2025 19:09:20</t>
+          <t>01.05.2025 20:27:55</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>9780321832054-1</t>
+          <t>9780321832054+1</t>
         </is>
       </c>
       <c r="G62" t="inlineStr"/>
@@ -2501,17 +2501,17 @@
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>registered</t>
+          <t>Registered</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>17.04.2025 19:09:21</t>
+          <t>01.05.2025 20:27:56</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>9780131118812-1</t>
+          <t>9780131118812+1</t>
         </is>
       </c>
       <c r="G63" t="inlineStr"/>
@@ -2534,17 +2534,17 @@
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>registered</t>
+          <t>Registered</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>17.04.2025 19:09:22</t>
+          <t>01.05.2025 20:27:57</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>9781716745522-1</t>
+          <t>9781716745522+1</t>
         </is>
       </c>
       <c r="G64" t="inlineStr"/>
@@ -2567,17 +2567,17 @@
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>registered</t>
+          <t>Registered</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>17.04.2025 19:09:22</t>
+          <t>01.05.2025 20:27:57</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>9781716745522-2</t>
+          <t>9781716745522+2</t>
         </is>
       </c>
       <c r="G65" t="inlineStr"/>
@@ -2600,17 +2600,17 @@
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>registered</t>
+          <t>Registered</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>17.04.2025 19:09:22</t>
+          <t>01.05.2025 20:27:58</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>9781716745522-3</t>
+          <t>9781716745522+3</t>
         </is>
       </c>
       <c r="G66" t="inlineStr"/>
@@ -2633,17 +2633,17 @@
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>registered</t>
+          <t>Registered</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>17.04.2025 19:09:23</t>
+          <t>01.05.2025 20:27:59</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>9781716745515-1</t>
+          <t>9781716745515+1</t>
         </is>
       </c>
       <c r="G67" t="inlineStr"/>
@@ -2666,17 +2666,17 @@
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>registered</t>
+          <t>Registered</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>17.04.2025 19:09:23</t>
+          <t>01.05.2025 20:28:00</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>9781716745515-2</t>
+          <t>9781716745515+2</t>
         </is>
       </c>
       <c r="G68" t="inlineStr"/>
@@ -2699,17 +2699,17 @@
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>registered</t>
+          <t>Registered</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>17.04.2025 19:09:24</t>
+          <t>01.05.2025 20:28:01</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
         <is>
-          <t>9781716745515-3</t>
+          <t>9781716745515+3</t>
         </is>
       </c>
       <c r="G69" t="inlineStr"/>
@@ -2732,17 +2732,17 @@
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>registered</t>
+          <t>Registered</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>17.04.2025 19:09:25</t>
+          <t>01.05.2025 20:28:03</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
         <is>
-          <t>9781259060489-2</t>
+          <t>9781259060489+2</t>
         </is>
       </c>
       <c r="G70" t="inlineStr"/>
@@ -2765,17 +2765,17 @@
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>registered</t>
+          <t>Registered</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>17.04.2025 19:09:26</t>
+          <t>01.05.2025 20:28:04</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
         <is>
-          <t>9780321546227-1</t>
+          <t>9780321546227+1</t>
         </is>
       </c>
       <c r="G71" t="inlineStr"/>
@@ -2798,17 +2798,17 @@
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>registered</t>
+          <t>Registered</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>17.04.2025 19:09:26</t>
+          <t>01.05.2025 20:28:05</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
         <is>
-          <t>9780321546227-2</t>
+          <t>9780321546227+2</t>
         </is>
       </c>
       <c r="G72" t="inlineStr"/>
@@ -2831,17 +2831,17 @@
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>registered</t>
+          <t>Registered</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>17.04.2025 19:09:27</t>
+          <t>01.05.2025 20:28:06</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
         <is>
-          <t>9780134670942-1</t>
+          <t>9780134670942+1</t>
         </is>
       </c>
       <c r="G73" t="inlineStr"/>
@@ -2864,17 +2864,17 @@
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>registered</t>
+          <t>Registered</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>17.04.2025 19:09:28</t>
+          <t>01.05.2025 20:28:07</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>9780138146269-1</t>
+          <t>9780138146269+1</t>
         </is>
       </c>
       <c r="G74" t="inlineStr"/>
@@ -2897,17 +2897,17 @@
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>registered</t>
+          <t>Registered</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>17.04.2025 19:09:28</t>
+          <t>01.05.2025 20:28:08</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>9780273771388-1</t>
+          <t>9780273771388+1</t>
         </is>
       </c>
       <c r="G75" t="inlineStr"/>

</xml_diff>